<commit_message>
update and compute dist_central instead of giving it as an input in the excel file
</commit_message>
<xml_diff>
--- a/Design/Test_excel.xlsx
+++ b/Design/Test_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabrina\Documents\GitHub\IRP-framework\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sabrina\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13496DDE-FB56-44D9-8E7E-1A8F4371EE49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549CB161-7B6A-47C0-852B-C5AD2D391239}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1357" yWindow="1080" windowWidth="19816" windowHeight="11895" activeTab="1" xr2:uid="{19BAF774-7CCA-4CA5-9E81-7F285EF3585C}"/>
+    <workbookView xWindow="10913" yWindow="8" windowWidth="19814" windowHeight="11895" activeTab="1" xr2:uid="{19BAF774-7CCA-4CA5-9E81-7F285EF3585C}"/>
   </bookViews>
   <sheets>
     <sheet name="Warehouses" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>fixed_cost</t>
-  </si>
-  <si>
-    <t>dist_central</t>
   </si>
 </sst>
 </file>
@@ -154,7 +151,7 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Tupel" xfId="1" xr:uid="{CF279EF5-48E9-448A-B4B6-3702B908129B}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="17">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -181,9 +178,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -223,8 +217,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{186F29CE-421F-48AF-B572-F32E8177B343}" name="Table_warehouses" displayName="Table_warehouses" ref="A1:H4" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A1:H4" xr:uid="{8E7FA2D4-CC0A-4297-A16C-2FD724E5FE08}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{186F29CE-421F-48AF-B572-F32E8177B343}" name="Table_warehouses" displayName="Table_warehouses" ref="A1:G4" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:G4" xr:uid="{8E7FA2D4-CC0A-4297-A16C-2FD724E5FE08}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -232,22 +226,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
     <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{ADA67064-CFCD-4FFB-B02E-A7CED971786A}" name="name" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{468CF79E-96CB-4679-9195-BC1FAFF46508}" name="latitude" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{DFBB2066-097E-4743-9CD9-3333FCDB2CE3}" name="longitude" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{E6658560-2E00-45F0-B0D7-B00FA8104A01}" name="lower" dataDxfId="13">
-      <calculatedColumnFormula>#REF!</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{45C8F503-9F29-4159-BC79-214688E2D2E4}" name="capacity" dataDxfId="12">
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{ADA67064-CFCD-4FFB-B02E-A7CED971786A}" name="name" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{468CF79E-96CB-4679-9195-BC1FAFF46508}" name="latitude" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{DFBB2066-097E-4743-9CD9-3333FCDB2CE3}" name="longitude" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{E6658560-2E00-45F0-B0D7-B00FA8104A01}" name="lower" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{45C8F503-9F29-4159-BC79-214688E2D2E4}" name="capacity" dataDxfId="11">
       <calculatedColumnFormula>2*Table_warehouses[[#This Row],[lower]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C1FF500B-DD53-402D-9187-132D4041E141}" name="initial" dataDxfId="11">
+    <tableColumn id="6" xr3:uid="{C1FF500B-DD53-402D-9187-132D4041E141}" name="initial" dataDxfId="10">
       <calculatedColumnFormula>Table_warehouses[[#This Row],[capacity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FDD1BB4E-4D33-4001-8CE7-239D39397497}" name="dist_central" dataDxfId="10"/>
     <tableColumn id="7" xr3:uid="{687DEC79-6075-4721-9E02-F2EABB245C1E}" name="fixed_cost" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -277,9 +267,7 @@
     <tableColumn id="5" xr3:uid="{7D8513EA-D80E-4ED2-AB7B-73C797AECE78}" name="capacity" dataDxfId="2">
       <calculatedColumnFormula>Table_schools[[#This Row],[consumption]]+2*Table_schools[[#This Row],[lower]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B8B21FBC-D7E8-414C-84CF-23BAFB0420EE}" name="initial" dataDxfId="1">
-      <calculatedColumnFormula>Table_schools[[#This Row],[capacity]]</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="6" xr3:uid="{B8B21FBC-D7E8-414C-84CF-23BAFB0420EE}" name="initial" dataDxfId="1"/>
     <tableColumn id="7" xr3:uid="{A1CD791A-52A2-42BE-B3B0-13710D29B045}" name="storage_cost" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -583,18 +571,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E97E7F-6D87-48CC-99F8-FA5AFD4F7868}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -614,13 +602,10 @@
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -644,11 +629,8 @@
       <c r="G2" s="3">
         <v>10</v>
       </c>
-      <c r="H2" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
@@ -670,13 +652,10 @@
         <v>300</v>
       </c>
       <c r="G3" s="3">
-        <v>4</v>
-      </c>
-      <c r="H3" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -698,9 +677,6 @@
         <v>260</v>
       </c>
       <c r="G4" s="3">
-        <v>8</v>
-      </c>
-      <c r="H4" s="3">
         <v>12</v>
       </c>
     </row>
@@ -887,7 +863,6 @@
         <v>27</v>
       </c>
       <c r="G6" s="3">
-        <f>Table_schools[[#This Row],[capacity]]</f>
         <v>27</v>
       </c>
       <c r="H6" s="3">
@@ -944,7 +919,6 @@
         <v>6</v>
       </c>
       <c r="G8" s="3">
-        <f>Table_schools[[#This Row],[capacity]]</f>
         <v>6</v>
       </c>
       <c r="H8" s="3">

</xml_diff>